<commit_message>
Fix(resistor-color): Table over main methode
</commit_message>
<xml_diff>
--- a/m-planification-jnltrav.xlsx
+++ b/m-planification-jnltrav.xlsx
@@ -610,11 +610,6 @@
         <v>× works if there is only very little time left (1 ms) × correctly handles orders that were started because there was time left (2 ms)</v>
       </c>
     </row>
-    <row r="19">
-      <c r="D19" t="str">
-        <v>DONE</v>
-      </c>
-    </row>
     <row r="20">
       <c r="A20" t="str">
         <v>Fix Door Policy</v>
@@ -625,9 +620,6 @@
       <c r="C20" t="str">
         <v>5</v>
       </c>
-      <c r="D20" t="str">
-        <v>DONE</v>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
@@ -734,18 +726,10 @@
         <v>WIP</v>
       </c>
     </row>
-    <row r="30">
-      <c r="D30" t="str">
-        <v>DONE</v>
-      </c>
-    </row>
     <row r="31">
       <c r="B31" t="str">
         <v>11/28/25</v>
       </c>
-      <c r="D31" t="str">
-        <v>DONE</v>
-      </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
@@ -813,18 +797,10 @@
         <v>DONE</v>
       </c>
     </row>
-    <row r="38">
-      <c r="D38" t="str">
-        <v>DONE</v>
-      </c>
-    </row>
     <row r="39">
       <c r="B39" t="str">
         <v>12/5/25</v>
       </c>
-      <c r="D39" t="str">
-        <v>DONE</v>
-      </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
@@ -870,28 +846,10 @@
         <v>DONE</v>
       </c>
     </row>
-    <row r="44">
-      <c r="D44" t="str">
-        <v>DONE</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="D45" t="str">
-        <v>DONE</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="D46" t="str">
-        <v>DONE</v>
-      </c>
-    </row>
     <row r="47">
       <c r="B47" t="str">
         <v>12/12/25</v>
       </c>
-      <c r="D47" t="str">
-        <v>DONE</v>
-      </c>
     </row>
     <row r="48">
       <c r="A48" t="str">
@@ -948,17 +906,9 @@
         <v>DONE</v>
       </c>
     </row>
-    <row r="53">
-      <c r="D53" t="str">
-        <v>DONE</v>
-      </c>
-    </row>
     <row r="54">
       <c r="B54" t="str">
         <v>12/19/25</v>
-      </c>
-      <c r="D54" t="str">
-        <v>DONE</v>
       </c>
     </row>
     <row r="55">

</xml_diff>